<commit_message>
added dynamic image category loading
</commit_message>
<xml_diff>
--- a/app/src/main/assets/Travel Phrases.xlsx
+++ b/app/src/main/assets/Travel Phrases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9732"/>
   </bookViews>
   <sheets>
     <sheet name="Phrases" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
   <si>
     <t>When does the flight leave?</t>
   </si>
@@ -123,6 +123,15 @@
   </si>
   <si>
     <t>Restaurant</t>
+  </si>
+  <si>
+    <t>file:///android_asset/airport.png</t>
+  </si>
+  <si>
+    <t>file:///android_asset/getting_around.png</t>
+  </si>
+  <si>
+    <t>file:///android_asset/restaurant.png</t>
   </si>
 </sst>
 </file>
@@ -440,20 +449,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="64.28515625" customWidth="1"/>
-    <col min="4" max="4" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.33203125" customWidth="1"/>
+    <col min="4" max="4" width="39.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -466,8 +476,11 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -480,8 +493,11 @@
       <c r="D2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -494,8 +510,11 @@
       <c r="D3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -508,8 +527,11 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
@@ -522,8 +544,11 @@
       <c r="D5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
@@ -536,8 +561,11 @@
       <c r="D6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7</v>
       </c>
@@ -550,8 +578,11 @@
       <c r="D7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
@@ -564,8 +595,11 @@
       <c r="D8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>9</v>
       </c>
@@ -578,8 +612,11 @@
       <c r="D9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10</v>
       </c>
@@ -592,8 +629,11 @@
       <c r="D10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>11</v>
       </c>
@@ -606,8 +646,11 @@
       <c r="D11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>12</v>
       </c>
@@ -620,8 +663,11 @@
       <c r="D12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>13</v>
       </c>
@@ -634,8 +680,11 @@
       <c r="D13" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>14</v>
       </c>
@@ -648,8 +697,11 @@
       <c r="D14" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>15</v>
       </c>
@@ -662,8 +714,12 @@
       <c r="D15" t="s">
         <v>29</v>
       </c>
+      <c r="E15" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>